<commit_message>
mise à jour journaux
</commit_message>
<xml_diff>
--- a/Documentation/Journeaux/OwnJournal de bord.xlsx
+++ b/Documentation/Journeaux/OwnJournal de bord.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7485"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7485" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="45">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -58,21 +58,12 @@
     <t>VIP</t>
   </si>
   <si>
-    <t>Realisation du Journal de bord et journal de travail</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>Realisation du premier exercice sur le moodle "Chandeleur"</t>
-  </si>
-  <si>
     <t>Intégrer une vraie fonction</t>
   </si>
   <si>
-    <t>Realisation du deuxième exercice sur le moodle "Recette"</t>
-  </si>
-  <si>
     <t>Optimiser au maximum les noms de variable. Utiliser les pointeurs mémoire avec les tableau x et le fonction</t>
   </si>
   <si>
@@ -161,6 +152,15 @@
   </si>
   <si>
     <t>Conception des uses cases</t>
+  </si>
+  <si>
+    <t>Réalisation du Journal de bord et journal de travail</t>
+  </si>
+  <si>
+    <t>Réalisation du premier exercice sur le moodle "Chandeleur"</t>
+  </si>
+  <si>
+    <t>Réalisation du deuxième exercice sur le moodle "Recette"</t>
   </si>
 </sst>
 </file>
@@ -333,7 +333,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -444,32 +444,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -555,6 +529,21 @@
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -563,7 +552,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -580,19 +569,13 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -607,13 +590,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="15" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -643,50 +620,47 @@
     <xf numFmtId="12" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="15" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="15" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="12" fontId="0" fillId="12" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="12" fontId="0" fillId="12" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="12" fontId="0" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="12" fontId="0" fillId="12" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="12" fontId="0" fillId="12" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -701,8 +675,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="15" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="15" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="15" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="15" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -716,7 +698,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1016,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="29.42578125" defaultRowHeight="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1027,369 +1009,419 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="50"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="47"/>
     </row>
     <row r="2" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="34" t="s">
+      <c r="C2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="13" t="s">
+      <c r="E2" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15">
+      <c r="B3" s="44">
+        <v>44229</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="30">
+        <v>0.75</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="44">
+        <v>44229</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="22">
+        <v>1</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="44">
+        <v>44230</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="44">
+        <v>44230</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="22">
+        <v>0.25</v>
+      </c>
+      <c r="E6" s="21"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="17"/>
+    </row>
+    <row r="7" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="44">
+        <v>44230</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="22">
+        <v>1</v>
+      </c>
+      <c r="E7" s="21"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="17"/>
+    </row>
+    <row r="8" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="44">
+        <v>44236</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="22">
+        <v>0.75</v>
+      </c>
+      <c r="E8" s="21"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="44">
+        <v>44236</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="22">
+        <v>0.25</v>
+      </c>
+      <c r="E9" s="21"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="17"/>
+    </row>
+    <row r="10" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="44">
+        <v>44237</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="17"/>
+    </row>
+    <row r="11" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="44">
+        <v>44238</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="17"/>
+    </row>
+    <row r="12" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="44">
+        <v>44240</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="17"/>
+    </row>
+    <row r="13" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="44">
         <v>44242</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="35">
-        <v>0.5</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="16">
+      <c r="C13" s="26"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="27"/>
+      <c r="B14" s="44">
+        <v>44243</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="42">
         <v>44244</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="G4" s="21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="16">
-        <v>44244</v>
-      </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="16">
+      <c r="C15" s="42"/>
+      <c r="D15" s="28">
+        <v>2.5</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="31"/>
+      <c r="G15" s="33"/>
+    </row>
+    <row r="16" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="13">
+        <v>44245</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="22">
+        <v>1</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="G16" s="32"/>
+    </row>
+    <row r="17" spans="2:7" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="13">
         <v>44246</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="21"/>
-    </row>
-    <row r="7" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="21"/>
-    </row>
-    <row r="8" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="21"/>
-    </row>
-    <row r="9" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="21"/>
-    </row>
-    <row r="10" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="21"/>
-    </row>
-    <row r="11" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="21"/>
-    </row>
-    <row r="12" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="21"/>
-    </row>
-    <row r="13" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="21"/>
-    </row>
-    <row r="14" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="32"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="16"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="38"/>
-    </row>
-    <row r="16" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="37"/>
-    </row>
-    <row r="17" spans="2:7" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="37"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="15"/>
+      <c r="G17" s="32"/>
     </row>
     <row r="18" spans="2:7" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="37"/>
+      <c r="B18" s="13">
+        <v>44249</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="15"/>
+      <c r="G18" s="32"/>
     </row>
     <row r="19" spans="2:7" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="37"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="32"/>
     </row>
     <row r="20" spans="2:7" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="37"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="32"/>
     </row>
     <row r="21" spans="2:7" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="37"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="32"/>
     </row>
     <row r="22" spans="2:7" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="37"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="32"/>
     </row>
     <row r="23" spans="2:7" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="42"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="37"/>
     </row>
     <row r="24" spans="2:7" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="42"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="37"/>
     </row>
     <row r="25" spans="2:7" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="42"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="37"/>
     </row>
     <row r="26" spans="2:7" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="42"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="37"/>
     </row>
     <row r="27" spans="2:7" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="42"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="37"/>
     </row>
     <row r="28" spans="2:7" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="42"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="37"/>
     </row>
     <row r="29" spans="2:7" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="42"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="37"/>
     </row>
     <row r="30" spans="2:7" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="42"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="37"/>
     </row>
     <row r="31" spans="2:7" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="41"/>
-      <c r="G31" s="42"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="37"/>
     </row>
     <row r="32" spans="2:7" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="42"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="37"/>
     </row>
     <row r="33" spans="2:7" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="42"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="36"/>
+      <c r="G33" s="37"/>
     </row>
     <row r="34" spans="2:7" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="42"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="37"/>
     </row>
     <row r="35" spans="2:7" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="40"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="42"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="37"/>
     </row>
     <row r="36" spans="2:7" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="41"/>
-      <c r="G36" s="42"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="37"/>
     </row>
     <row r="37" spans="2:7" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="31"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="41"/>
-      <c r="G37" s="42"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="36"/>
+      <c r="G37" s="37"/>
     </row>
     <row r="38" spans="2:7" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="31"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="40"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="42"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="37"/>
     </row>
     <row r="39" spans="2:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="39"/>
-      <c r="C39" s="39"/>
-      <c r="D39" s="40"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="41"/>
-      <c r="G39" s="42"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="37"/>
     </row>
     <row r="41" spans="2:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="43" t="s">
-        <v>28</v>
-      </c>
-      <c r="C41" s="43"/>
-      <c r="D41" s="44">
+      <c r="B41" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="38"/>
+      <c r="D41" s="39">
         <f>SUM(D13:D38)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1415,10 +1447,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F16"/>
+  <dimension ref="B1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="29.28515625" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1428,19 +1460,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="52"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="49"/>
     </row>
     <row r="2" spans="2:6" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="18" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -1455,174 +1487,426 @@
     </row>
     <row r="3" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="43">
+        <v>44229</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>40</v>
+      <c r="F3" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="C4" s="43">
+        <v>44229</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="C5" s="43">
+        <v>44230</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="C6" s="43">
+        <v>44230</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="43">
+        <v>44230</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="43">
+        <v>44236</v>
+      </c>
+      <c r="D8" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="43">
+        <v>44236</v>
+      </c>
+      <c r="D9" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="6"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="28" t="s">
+      <c r="E9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="43">
+        <v>44237</v>
+      </c>
+      <c r="D10" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="6"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="28" t="s">
+      <c r="E10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="43">
+        <v>44238</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="6"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="6"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>40</v>
+      <c r="F11" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="7"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="10" t="s">
-        <v>40</v>
+      <c r="B12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="43">
+        <v>44240</v>
+      </c>
+      <c r="D12" s="25"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="7"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="10" t="s">
-        <v>40</v>
+      <c r="B13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="43">
+        <v>44242</v>
+      </c>
+      <c r="D13" s="25"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="7"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="10" t="s">
-        <v>40</v>
+      <c r="B14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="43">
+        <v>44243</v>
+      </c>
+      <c r="D14" s="25"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="7"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="10" t="s">
-        <v>40</v>
+      <c r="B15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="43">
+        <v>44244</v>
+      </c>
+      <c r="D15" s="25"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="7"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="10" t="s">
-        <v>40</v>
+      <c r="B16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="43">
+        <v>44245</v>
+      </c>
+      <c r="D16" s="25"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="43">
+        <v>44246</v>
+      </c>
+      <c r="D17" s="25"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="43">
+        <v>44247</v>
+      </c>
+      <c r="D18" s="25"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="43">
+        <v>44248</v>
+      </c>
+      <c r="D19" s="25"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="43">
+        <v>44249</v>
+      </c>
+      <c r="D20" s="25"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="43">
+        <v>44250</v>
+      </c>
+      <c r="D21" s="25"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="43">
+        <v>44251</v>
+      </c>
+      <c r="D22" s="25"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="43">
+        <v>44252</v>
+      </c>
+      <c r="D23" s="25"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="43">
+        <v>44253</v>
+      </c>
+      <c r="D24" s="25"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="43">
+        <v>44254</v>
+      </c>
+      <c r="D25" s="25"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="43"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="43">
+        <v>44256</v>
+      </c>
+      <c r="D27" s="25"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="43">
+        <v>44257</v>
+      </c>
+      <c r="D28" s="25"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="43">
+        <v>44258</v>
+      </c>
+      <c r="D29" s="25"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="43">
+        <v>44259</v>
+      </c>
+      <c r="D30" s="25"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="43">
+        <v>44260</v>
+      </c>
+      <c r="D31" s="25"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="43">
+        <v>44261</v>
+      </c>
+      <c r="D32" s="25"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1648,48 +1932,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="40" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="41" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="41" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="41" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="46" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="41" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="41" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="46" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="46" t="s">
-        <v>36</v>
-      </c>
-    </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="46" t="s">
-        <v>37</v>
+      <c r="A9" s="41" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>